<commit_message>
inserindo menu do inventário
</commit_message>
<xml_diff>
--- a/LIBERADO.xlsx
+++ b/LIBERADO.xlsx
@@ -48,14 +48,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0000000000"/>
     <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="168" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="@"/>
-    <numFmt numFmtId="170" formatCode="0.00&quot;mi&quot;"/>
+    <numFmt numFmtId="169" formatCode="#,##0.00"/>
+    <numFmt numFmtId="170" formatCode="@"/>
+    <numFmt numFmtId="171" formatCode="0.00&quot;mi&quot;"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -259,7 +260,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -267,7 +268,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -287,7 +288,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -318,9 +319,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>608760</xdr:colOff>
+      <xdr:colOff>608400</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>370440</xdr:rowOff>
+      <xdr:rowOff>370080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -335,7 +336,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8501040" y="9639360"/>
-          <a:ext cx="8280" cy="8280"/>
+          <a:ext cx="7920" cy="7920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -358,8 +359,8 @@
   </sheetPr>
   <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AMJ2" activeCellId="0" sqref="AMJ2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="true" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
ajustando o qrcode da etiqueta
</commit_message>
<xml_diff>
--- a/LIBERADO.xlsx
+++ b/LIBERADO.xlsx
@@ -257,7 +257,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="170" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -319,9 +319,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>608040</xdr:colOff>
+      <xdr:colOff>607680</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>369720</xdr:rowOff>
+      <xdr:rowOff>369360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -335,8 +335,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8501040" y="9639360"/>
-          <a:ext cx="7560" cy="7560"/>
+          <a:off x="8501040" y="9636840"/>
+          <a:ext cx="7200" cy="7200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -359,8 +359,8 @@
   </sheetPr>
   <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="true" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -372,10 +372,10 @@
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1024" min="8" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="105" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="71.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="91" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>50490762</v>
       </c>

</xml_diff>